<commit_message>
feat: add 'icon' field to schema and update some field names
</commit_message>
<xml_diff>
--- a/db/db.xlsx
+++ b/db/db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim Gwan Ju\WebstormProjects\websys\server\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9537BB52-DC5D-4B0E-9965-FB759C16ECA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C605DD-3E70-4BA9-8585-CBE5DEECB1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1CF454AA-EBAE-4977-B105-BA28832D8967}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{1CF454AA-EBAE-4977-B105-BA28832D8967}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="8" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -307,6 +307,22 @@
   </si>
   <si>
     <t>2023-11-20T10:20:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팔달관 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다산관 1층</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구학생회관 1층</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -701,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52912C7-1CC3-4D5B-B8C3-A6158BD4E487}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1034,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0A22A8-9713-402E-97DB-804A368BD412}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1050,7 +1066,7 @@
     <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1063,8 +1079,11 @@
       <c r="D1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1077,8 +1096,11 @@
       <c r="D2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1091,8 +1113,11 @@
       <c r="D3">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1105,8 +1130,11 @@
       <c r="D4">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1119,8 +1147,11 @@
       <c r="D5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1133,8 +1164,11 @@
       <c r="D6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1147,8 +1181,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1160,6 +1197,9 @@
       </c>
       <c r="D8">
         <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>